<commit_message>
Validation of existing spreadsheets and changing of mapping to HRC requirement TOPMED
</commit_message>
<xml_diff>
--- a/Snplists/CD_GRS42/CD_GRS42_1000G_nopalin_pos_hg19.xlsx
+++ b/Snplists/CD_GRS42/CD_GRS42_1000G_nopalin_pos_hg19.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universityofexeteruk-my.sharepoint.com/personal/s_sharp_exeter_ac_uk/Documents/LIVE/hla-prs-toolkit/Snplists/CD_GRS42/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="301" documentId="13_ncr:1_{247850E2-87A2-334F-8E57-962B47D46C51}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{D63CA6F6-558E-C14A-9A41-58B0060088CE}"/>
+  <xr:revisionPtr revIDLastSave="311" documentId="13_ncr:1_{247850E2-87A2-334F-8E57-962B47D46C51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5A87D74D-228B-FD4D-BC75-BDC2B061EB31}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="460" windowWidth="14400" windowHeight="16500" xr2:uid="{790D5DEB-C308-234D-BB35-18DFB1DC5B15}"/>
+    <workbookView xWindow="26300" yWindow="2840" windowWidth="23740" windowHeight="23560" xr2:uid="{790D5DEB-C308-234D-BB35-18DFB1DC5B15}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -714,8 +714,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2936C92A-3A1B-4C43-81CA-C5EF6A570C1B}">
   <dimension ref="A1:P1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="G34" sqref="G34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L27" sqref="L27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -826,7 +826,9 @@
       <c r="J3" s="1" t="s">
         <v>59</v>
       </c>
+      <c r="N3" s="1"/>
       <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
@@ -1804,9 +1806,6 @@
       <c r="J31" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="N31" s="1"/>
-      <c r="O31" s="1"/>
-      <c r="P31" s="1"/>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">

</xml_diff>